<commit_message>
added Orders Flow code
</commit_message>
<xml_diff>
--- a/resources/PlaceOrder/PlaceOrder.xlsx
+++ b/resources/PlaceOrder/PlaceOrder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win10\eclipse-workspace\FirstTestNG\resources\PlaceOrder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2ED8F7-BE1E-4A8B-81D9-E0C30801609A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48236D3F-7687-4C44-973E-67ED18753877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +332,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -445,6 +451,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +739,7 @@
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +754,7 @@
       <c r="A1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="16">
         <v>2</v>
       </c>
       <c r="C1" s="4"/>
@@ -983,20 +994,20 @@
       <c r="A13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="17">
         <v>2</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="17">
         <v>2</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1408,7 +1419,7 @@
       <c r="A52" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="18">
         <v>2</v>
       </c>
     </row>

</xml_diff>